<commit_message>
Modified ExcelDataProvider to read only based on must read column
</commit_message>
<xml_diff>
--- a/src/test/resources/data/data.xlsx
+++ b/src/test/resources/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Username</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>z98765</t>
+  </si>
+  <si>
+    <t>Must Read</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -396,36 +405,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>